<commit_message>
test related to fdo#51601
Change-Id: If1edd974ba81f56b0ff32ffe0bfd376bb370943b
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/bug-fixes.xlsx
+++ b/sc/qa/unit/data/xlsx/bug-fixes.xlsx
@@ -9,13 +9,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Sheet Number</t>
   </si>
@@ -30,6 +31,9 @@
   </si>
   <si>
     <t>Contains summary</t>
+  </si>
+  <si>
+    <t>Fdo#51601</t>
   </si>
 </sst>
 </file>
@@ -42,6 +46,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -125,17 +130,18 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+      <selection activeCell="D4" activeCellId="0" pane="topLeft" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3647058823529"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0588235294118"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.521568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.7294117647059"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.2666666666667"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="0" width="11.7294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.5921568627451"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -146,7 +152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -157,17 +163,20 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -181,4 +190,36 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="C1"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C1" activeCellId="0" pane="topLeft" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="C1" s="0" t="e">
+        <f aca="false">averageif(A2:B2)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>